<commit_message>
chose location and created map
</commit_message>
<xml_diff>
--- a/data/car_wash_costs.xlsx
+++ b/data/car_wash_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evanr\Documents\NSS\Projects\Car-Wash-Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7E3BA4-AE08-4485-9EDD-C500D567B7B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E6FC35-1F6E-4F49-857F-3A6A1C407E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{541C1CEF-9207-4DFC-BA7A-2496AF5DA057}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>start_up_costs</t>
   </si>
@@ -105,40 +105,52 @@
     <t>weekly_gross_income</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>monthly_gross_income</t>
   </si>
   <si>
     <t>yearly_gross_income</t>
   </si>
   <si>
-    <t>Sullivan</t>
-  </si>
-  <si>
-    <t>weekly_expenses</t>
-  </si>
-  <si>
-    <t>cost to wash each car</t>
-  </si>
-  <si>
     <t>daily_cost</t>
   </si>
   <si>
-    <t>employees</t>
-  </si>
-  <si>
-    <t>hourly_wage</t>
-  </si>
-  <si>
-    <t>total_hours_worked</t>
-  </si>
-  <si>
-    <t>hours_worked_per_employee</t>
-  </si>
-  <si>
-    <t>employee_pay</t>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>natural gas</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>detergents/chemicals</t>
+  </si>
+  <si>
+    <t>repairs/maintenance</t>
+  </si>
+  <si>
+    <t>administrative expenses</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>expenses_per_car</t>
+  </si>
+  <si>
+    <t>county</t>
+  </si>
+  <si>
+    <t>employee pay</t>
+  </si>
+  <si>
+    <t>total_expenses</t>
+  </si>
+  <si>
+    <t>cost</t>
   </si>
 </sst>
 </file>
@@ -205,7 +217,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -226,6 +238,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -544,17 +559,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7792ED2-222D-4C74-8776-FC877525331E}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="1"/>
+    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="1" bestFit="1" customWidth="1"/>
@@ -563,8 +580,8 @@
     <col min="12" max="12" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -576,7 +593,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>17</v>
@@ -597,16 +614,16 @@
         <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -614,46 +631,45 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>200000</v>
+        <v>75000</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="1">
-        <v>20210</v>
+        <v>18510</v>
       </c>
       <c r="G2" s="1">
         <v>8.2900000000000005E-3</v>
       </c>
       <c r="H2" s="1">
         <f>SUM(F2*G2)</f>
-        <v>167.54090000000002</v>
+        <v>153.4479</v>
       </c>
       <c r="I2" s="1">
         <v>15</v>
       </c>
       <c r="J2" s="1">
         <f>SUM(H2*I2)</f>
-        <v>2513.1135000000004</v>
+        <v>2301.7184999999999</v>
       </c>
       <c r="K2" s="1">
         <f>SUM(J2*7)</f>
-        <v>17591.794500000004</v>
+        <v>16112.029500000001</v>
       </c>
       <c r="L2" s="1">
         <f>SUM(K2*4)</f>
-        <v>70367.178000000014</v>
+        <v>64448.118000000002</v>
       </c>
       <c r="M2" s="1">
-        <f>SUM(L2*12)</f>
-        <v>844406.13600000017</v>
+        <f>SUM(J2*350)</f>
+        <v>805601.47499999998</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="1">
-        <f>SUM(H2*4.13)</f>
-        <v>691.94391700000006</v>
+        <v>27</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -661,14 +677,13 @@
         <v>9</v>
       </c>
       <c r="B3" s="2">
-        <v>2900</v>
+        <v>2184</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="1">
-        <f>SUM(N12*L12)</f>
-        <v>1701</v>
+        <v>28</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.12</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -676,7 +691,13 @@
         <v>10</v>
       </c>
       <c r="B4" s="2">
-        <v>50</v>
+        <v>25</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.16</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -686,13 +707,25 @@
       <c r="B5" s="2">
         <v>300</v>
       </c>
+      <c r="O5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.64</v>
+      </c>
     </row>
     <row r="6" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="2">
-        <v>30000</v>
+        <v>36400</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0.47</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,7 +733,13 @@
         <v>2</v>
       </c>
       <c r="B7" s="2">
-        <v>200000</v>
+        <v>250000</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -710,21 +749,40 @@
       <c r="B8" s="2">
         <v>185000</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="2">
         <v>211000</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="5">
+        <f>SUM(P2:P8)</f>
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2">
-        <v>12100</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -734,18 +792,6 @@
       <c r="B11" s="2">
         <v>20000</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>32</v>
-      </c>
     </row>
     <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -754,19 +800,6 @@
       <c r="B12" s="2">
         <v>5000</v>
       </c>
-      <c r="K12" s="1">
-        <v>6</v>
-      </c>
-      <c r="L12" s="1">
-        <v>9</v>
-      </c>
-      <c r="M12" s="1">
-        <v>31.5</v>
-      </c>
-      <c r="N12" s="1">
-        <f>SUM(M12*K12)</f>
-        <v>189</v>
-      </c>
     </row>
     <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -783,6 +816,7 @@
       <c r="B14" s="2">
         <v>5000</v>
       </c>
+      <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -791,6 +825,7 @@
       <c r="B15" s="2">
         <v>6000</v>
       </c>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
@@ -798,10 +833,26 @@
       </c>
       <c r="B16" s="5">
         <f>SUM(B2:B15)</f>
-        <v>887350</v>
-      </c>
-    </row>
-    <row r="17" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+        <v>815909</v>
+      </c>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="11:12" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="11:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="11:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K19" s="2"/>
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="11:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="11:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K21" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
read in demographics, completed start up costs
</commit_message>
<xml_diff>
--- a/data/car_wash_costs.xlsx
+++ b/data/car_wash_costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evanr\Documents\NSS\Projects\Car-Wash-Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E6FC35-1F6E-4F49-857F-3A6A1C407E6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C01D36E-0667-4193-BF3B-9308C590D767}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{541C1CEF-9207-4DFC-BA7A-2496AF5DA057}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="16440" xr2:uid="{541C1CEF-9207-4DFC-BA7A-2496AF5DA057}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>start_up_costs</t>
   </si>
@@ -111,9 +111,6 @@
     <t>yearly_gross_income</t>
   </si>
   <si>
-    <t>daily_cost</t>
-  </si>
-  <si>
     <t>Washington</t>
   </si>
   <si>
@@ -151,14 +148,79 @@
   </si>
   <si>
     <t>cost</t>
+  </si>
+  <si>
+    <t>monthly_cost</t>
+  </si>
+  <si>
+    <t>annual_cost</t>
+  </si>
+  <si>
+    <t>average_hours_per_day</t>
+  </si>
+  <si>
+    <t>hourly_rate</t>
+  </si>
+  <si>
+    <t>num_of_employees</t>
+  </si>
+  <si>
+    <t>daily_empl_expense</t>
+  </si>
+  <si>
+    <t>total_hours_per_day</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>detergent/chemicals</t>
+  </si>
+  <si>
+    <t>repairs/maintanence</t>
+  </si>
+  <si>
+    <t>adminstrative expenses</t>
+  </si>
+  <si>
+    <t>total_per day</t>
+  </si>
+  <si>
+    <t>loan</t>
+  </si>
+  <si>
+    <t>expenses</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>total profit</t>
+  </si>
+  <si>
+    <t>total expenses</t>
+  </si>
+  <si>
+    <t>gross income</t>
+  </si>
+  <si>
+    <t>Profit Margin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -192,7 +254,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -211,13 +273,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -225,28 +313,57 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="4" builtinId="5"/>
     <cellStyle name="Total" xfId="2" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,299 +676,543 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7792ED2-222D-4C74-8776-FC877525331E}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="23.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="17" max="17" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>75000</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="14">
+        <v>18510</v>
+      </c>
+      <c r="G2" s="11">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H2" s="11">
+        <f>SUM(F2*G2)</f>
+        <v>74.040000000000006</v>
+      </c>
+      <c r="I2" s="12">
+        <v>15</v>
+      </c>
+      <c r="J2" s="12">
+        <f>SUM(H2*I2)</f>
+        <v>1110.6000000000001</v>
+      </c>
+      <c r="K2" s="12">
+        <f>SUM(J2*7)</f>
+        <v>7774.2000000000007</v>
+      </c>
+      <c r="L2" s="12">
+        <f>SUM(K2*4)</f>
+        <v>31096.800000000003</v>
+      </c>
+      <c r="M2" s="12">
+        <f>SUM(J2*350)</f>
+        <v>388710.00000000006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="12">
+        <v>2184</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="12">
+        <v>300</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="12">
+        <v>40000</v>
+      </c>
+      <c r="E6" s="7">
+        <v>8</v>
+      </c>
+      <c r="F6" s="7">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="G6" s="7">
+        <f>SUM(F6*4)</f>
+        <v>34.520000000000003</v>
+      </c>
+      <c r="H6" s="15">
+        <v>9</v>
+      </c>
+      <c r="I6" s="15">
+        <f>SUM(G6*H6)</f>
+        <v>310.68</v>
+      </c>
+      <c r="J6" s="15">
+        <f>SUM(I6*7)</f>
+        <v>2174.7600000000002</v>
+      </c>
+      <c r="K6" s="15">
+        <f>SUM(I6*29.2)</f>
+        <v>9071.8559999999998</v>
+      </c>
+      <c r="L6" s="15">
+        <f>SUM(I6*365)</f>
+        <v>113398.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="12">
+        <v>185000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="12">
+        <v>211000</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="12">
+        <v>10000</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="12">
+        <v>-0.5</v>
+      </c>
+      <c r="G10" s="16">
+        <f>SUM(F10*$H$2)</f>
+        <v>-37.020000000000003</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="16">
+        <f>SUM(G10*29.2)</f>
+        <v>-1080.9840000000002</v>
+      </c>
+      <c r="L10" s="16">
+        <f>SUM(G10*350)</f>
+        <v>-12957.000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="12">
+        <v>20000</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="12">
+        <v>-0.12</v>
+      </c>
+      <c r="G11" s="16">
+        <f t="shared" ref="G11:G17" si="0">SUM(F11*$H$2)</f>
+        <v>-8.8848000000000003</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="16">
+        <f>SUM(G11*29.2)</f>
+        <v>-259.43616000000003</v>
+      </c>
+      <c r="L11" s="16">
+        <f>SUM(G11*350)</f>
+        <v>-3109.6800000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="12">
+        <v>5000</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="12">
+        <v>-0.16</v>
+      </c>
+      <c r="G12" s="16">
+        <f t="shared" si="0"/>
+        <v>-11.846400000000001</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="16">
+        <f>SUM(G12*29.2)</f>
+        <v>-345.91488000000004</v>
+      </c>
+      <c r="L12" s="16">
+        <f>SUM(G12*350)</f>
+        <v>-4146.2400000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12">
+        <v>10000</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="12">
+        <v>-0.64</v>
+      </c>
+      <c r="G13" s="16">
+        <f t="shared" si="0"/>
+        <v>-47.385600000000004</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="16">
+        <f>SUM(G13*29.2)</f>
+        <v>-1383.6595200000002</v>
+      </c>
+      <c r="L13" s="16">
+        <f>SUM(G13*350)</f>
+        <v>-16584.960000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="12">
+        <v>5000</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="12">
+        <v>-0.47</v>
+      </c>
+      <c r="G14" s="16">
+        <f t="shared" si="0"/>
+        <v>-34.7988</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K14" s="16">
+        <f>SUM(G14*29.2)</f>
+        <v>-1016.12496</v>
+      </c>
+      <c r="L14" s="16">
+        <f>SUM(G14*350)</f>
+        <v>-12179.58</v>
+      </c>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="12">
+        <v>40000</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="12">
+        <v>-1</v>
+      </c>
+      <c r="G15" s="16">
+        <f t="shared" si="0"/>
+        <v>-74.040000000000006</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K15" s="16">
+        <f>SUM(G15*29.2)</f>
+        <v>-2161.9680000000003</v>
+      </c>
+      <c r="L15" s="16">
+        <f>SUM(G15*350)</f>
+        <v>-25914.000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="12">
+        <v>6024</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2">
-        <v>75000</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="1">
-        <v>18510</v>
-      </c>
-      <c r="G2" s="1">
-        <v>8.2900000000000005E-3</v>
-      </c>
-      <c r="H2" s="1">
-        <f>SUM(F2*G2)</f>
-        <v>153.4479</v>
-      </c>
-      <c r="I2" s="1">
-        <v>15</v>
-      </c>
-      <c r="J2" s="1">
-        <f>SUM(H2*I2)</f>
-        <v>2301.7184999999999</v>
-      </c>
-      <c r="K2" s="1">
-        <f>SUM(J2*7)</f>
-        <v>16112.029500000001</v>
-      </c>
-      <c r="L2" s="1">
-        <f>SUM(K2*4)</f>
-        <v>64448.118000000002</v>
-      </c>
-      <c r="M2" s="1">
-        <f>SUM(J2*350)</f>
-        <v>805601.47499999998</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2">
-        <v>2184</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2">
-        <v>25</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="2">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2">
-        <v>300</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="2">
-        <v>36400</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2">
-        <v>250000</v>
-      </c>
-      <c r="O7" s="1" t="s">
+      <c r="F16" s="12">
+        <v>-2.02</v>
+      </c>
+      <c r="G16" s="16">
+        <f t="shared" si="0"/>
+        <v>-149.5608</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" s="16">
+        <v>-9071.8559999999998</v>
+      </c>
+      <c r="L16" s="16">
+        <v>-113398.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="4">
+        <f>SUM(B2:B16)</f>
+        <v>859533</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2">
-        <v>185000</v>
-      </c>
-      <c r="O8" s="1" t="s">
+      <c r="F17" s="8">
+        <f>SUM(F10:F16)</f>
+        <v>-4.91</v>
+      </c>
+      <c r="G17" s="8">
+        <f t="shared" si="0"/>
+        <v>-363.53640000000001</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" s="12">
+        <v>-4850</v>
+      </c>
+      <c r="L17" s="16">
+        <f>SUM(K17*12)</f>
+        <v>-58200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="2">
-        <v>1.58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2">
-        <v>211000</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="P9" s="5">
-        <f>SUM(P2:P8)</f>
-        <v>4.47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2">
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2">
-        <v>5000</v>
-      </c>
-      <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2">
-        <v>6000</v>
-      </c>
-      <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="5">
-        <f>SUM(B2:B15)</f>
-        <v>815909</v>
-      </c>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="11:12" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="11:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="11:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K18" s="8">
+        <f>SUM(K10:K17)</f>
+        <v>-20169.943520000001</v>
+      </c>
+      <c r="L18" s="8">
+        <f>SUM(L10:L17)</f>
+        <v>-246489.66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="K19" s="2"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="11:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="11:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K21" s="2"/>
+    <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="12">
+        <f>M2</f>
+        <v>388710.00000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="H23" s="12">
+        <f>L18</f>
+        <v>-246489.66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="2"/>
+      <c r="G24" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" s="15">
+        <f>SUM(H22:H23)</f>
+        <v>142220.34000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="2"/>
+      <c r="G26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="17">
+        <f>SUM((388710-246489.66)/H22)</f>
+        <v>0.365877749479046</v>
+      </c>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added references to powerpoint
</commit_message>
<xml_diff>
--- a/data/car_wash_costs.xlsx
+++ b/data/car_wash_costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evanr\Documents\NSS\Projects\Car-Wash-Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08C4BB8-6077-4E49-908F-6E43211B9A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17536127-A4A3-46F9-AFC4-E3B85C22CA11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{541C1CEF-9207-4DFC-BA7A-2496AF5DA057}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="16440" xr2:uid="{541C1CEF-9207-4DFC-BA7A-2496AF5DA057}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -673,7 +673,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added sections to presentation, minor adjustments
</commit_message>
<xml_diff>
--- a/data/car_wash_costs.xlsx
+++ b/data/car_wash_costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evanr\Documents\NSS\Projects\Car-Wash-Capstone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17536127-A4A3-46F9-AFC4-E3B85C22CA11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9EC523-1356-4A91-AC6E-17EE89BBF9F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="16440" xr2:uid="{541C1CEF-9207-4DFC-BA7A-2496AF5DA057}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
   <si>
     <t>start_up_costs</t>
   </si>
@@ -87,9 +87,6 @@
     <t>AADT</t>
   </si>
   <si>
-    <t>capture rate</t>
-  </si>
-  <si>
     <t>daily_washes</t>
   </si>
   <si>
@@ -132,18 +129,12 @@
     <t>total</t>
   </si>
   <si>
-    <t>expenses_per_car</t>
-  </si>
-  <si>
     <t>county</t>
   </si>
   <si>
     <t>employee pay</t>
   </si>
   <si>
-    <t>cost</t>
-  </si>
-  <si>
     <t>monthly_cost</t>
   </si>
   <si>
@@ -183,18 +174,12 @@
     <t>adminstrative expenses</t>
   </si>
   <si>
-    <t>total_per day</t>
-  </si>
-  <si>
     <t>loan</t>
   </si>
   <si>
     <t>expenses</t>
   </si>
   <si>
-    <t>Equipment</t>
-  </si>
-  <si>
     <t>total profit</t>
   </si>
   <si>
@@ -205,6 +190,24 @@
   </si>
   <si>
     <t>Profit Margin</t>
+  </si>
+  <si>
+    <t>Misc. Equipment</t>
+  </si>
+  <si>
+    <t>capture_rate</t>
+  </si>
+  <si>
+    <t>Expenses</t>
+  </si>
+  <si>
+    <t>Cost Per Car</t>
+  </si>
+  <si>
+    <t>Daily Total</t>
+  </si>
+  <si>
+    <t>Employee Pay (1-Year)</t>
   </si>
 </sst>
 </file>
@@ -299,7 +302,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -351,6 +354,12 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -673,7 +682,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection sqref="A1:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -705,31 +714,31 @@
         <v>8</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -740,7 +749,7 @@
         <v>75000</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="14">
         <v>18510</v>
@@ -796,28 +805,28 @@
         <v>300</v>
       </c>
       <c r="E5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="9" t="s">
+      <c r="K5" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -853,8 +862,8 @@
         <v>11339.82</v>
       </c>
       <c r="L6" s="15">
-        <f>SUM(I6*365)</f>
-        <v>141747.75</v>
+        <f>SUM(I6*350)</f>
+        <v>135922.5</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -881,22 +890,22 @@
         <v>211000</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>49</v>
+        <v>54</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>56</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -907,7 +916,7 @@
         <v>10000</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="12">
         <v>-0.5</v>
@@ -917,7 +926,7 @@
         <v>-37.020000000000003</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K10" s="16">
         <f t="shared" ref="K10:K15" si="0">SUM(G10*29.2)</f>
@@ -936,7 +945,7 @@
         <v>20000</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="12">
         <v>-0.12</v>
@@ -946,7 +955,7 @@
         <v>-8.8848000000000003</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K11" s="16">
         <f t="shared" si="0"/>
@@ -965,7 +974,7 @@
         <v>5000</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="12">
         <v>-0.16</v>
@@ -975,7 +984,7 @@
         <v>-11.846400000000001</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K12" s="16">
         <f t="shared" si="0"/>
@@ -994,7 +1003,7 @@
         <v>10000</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="12">
         <v>-0.64</v>
@@ -1004,7 +1013,7 @@
         <v>-47.385600000000004</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="K13" s="16">
         <f t="shared" si="0"/>
@@ -1023,7 +1032,7 @@
         <v>5000</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="12">
         <v>-0.47</v>
@@ -1033,7 +1042,7 @@
         <v>-34.7988</v>
       </c>
       <c r="J14" s="11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="K14" s="16">
         <f t="shared" si="0"/>
@@ -1047,13 +1056,13 @@
     </row>
     <row r="15" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B15" s="12">
-        <v>40000</v>
+        <v>135000</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="12">
         <v>-1</v>
@@ -1063,7 +1072,7 @@
         <v>-74.040000000000006</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="K15" s="16">
         <f t="shared" si="0"/>
@@ -1076,13 +1085,13 @@
     </row>
     <row r="16" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="B16" s="12">
-        <v>6024</v>
+        <v>40000</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" s="12">
         <v>-5.24513776337115</v>
@@ -1092,25 +1101,24 @@
         <v>-388.34999999999997</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K16" s="16">
         <v>-11339.82</v>
       </c>
       <c r="L16" s="16">
-        <v>-141747.75</v>
+        <v>-135922.5</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="4">
-        <f>SUM(B2:B16)</f>
-        <v>859533</v>
+      <c r="A17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="12">
+        <v>6024</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F17" s="8">
         <f>SUM(F10:F16)</f>
@@ -1121,7 +1129,7 @@
         <v>-602.32560000000001</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="K17" s="12">
         <v>-4850</v>
@@ -1132,8 +1140,15 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="4">
+        <f>SUM(B2:B17)</f>
+        <v>994533</v>
+      </c>
       <c r="J18" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="K18" s="8">
         <f>SUM(K10:K17)</f>
@@ -1141,11 +1156,11 @@
       </c>
       <c r="L18" s="8">
         <f>SUM(L10:L17)</f>
-        <v>-274839.21000000002</v>
+        <v>-269013.96000000002</v>
       </c>
       <c r="M18" s="5">
         <f>SUM(L18*-1)</f>
-        <v>274839.21000000002</v>
+        <v>269013.96000000002</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1157,7 +1172,7 @@
     </row>
     <row r="22" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G22" s="11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="H22" s="12">
         <f>M2</f>
@@ -1166,21 +1181,21 @@
     </row>
     <row r="23" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G23" s="11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H23" s="12">
         <f>L18</f>
-        <v>-274839.21000000002</v>
+        <v>-269013.96000000002</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F24" s="2"/>
       <c r="G24" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="H24" s="15">
         <f>SUM(H22:H23)</f>
-        <v>113870.79000000004</v>
+        <v>119696.04000000004</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1189,11 +1204,11 @@
     <row r="26" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26" s="2"/>
       <c r="G26" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H26" s="17">
         <f>SUM((H22-M18)/H22)</f>
-        <v>0.29294535772169489</v>
+        <v>0.30793146561704104</v>
       </c>
       <c r="M26" s="5"/>
     </row>

</xml_diff>